<commit_message>
handling any username + password + bill if not entered beforehand into config params
</commit_message>
<xml_diff>
--- a/Fall25_Bills_Budget.xlsx
+++ b/Fall25_Bills_Budget.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault.sharepoint.com/sites/MarineRoboticsGroup/Shared Documents/OPS-1 Operations/Fall 2025 Finances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5320689-27C0-4790-B207-2A98E27EB644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{22ADE271-ECDF-4993-AB45-163730D1AD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="78">
   <si>
     <t>Bill No.</t>
   </si>
@@ -135,6 +135,48 @@
   </si>
   <si>
     <t>https://gtvault.sharepoint.com/sites/MarineRoboticsGroup/Shared%20Documents/Forms/AllItems.aspx?viewid=fd287ec4%2D27e7%2D4522%2Da3ab%2Dc8258347670f&amp;id=%2Fsites%2FMarineRoboticsGroup%2FShared%20Documents%2FOPS%2D1%20Operations%2FFall%202025%20Finances%2FFall%202025%20Bill%20Proof%2FMarine%20Robotics%20Group%20Fall%202025%20Bill%20No%2E%201%2FFlag%2Epng&amp;parent=%2Fsites%2FMarineRoboticsGroup%2FShared%20Documents%2FOPS%2D1%20Operations%2FFall%202025%20Finances%2FFall%202025%20Bill%20Proof%2FMarine%20Robotics%20Group%20Fall%202025%20Bill%20No%2E%201</t>
+  </si>
+  <si>
+    <t>Low Profile 8020</t>
+  </si>
+  <si>
+    <t>mcmaster</t>
+  </si>
+  <si>
+    <t>48"x1"x0.5" 8020 low profile rail; Used for building robot and testing structures</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/47065T68-47065T682/</t>
+  </si>
+  <si>
+    <t>Low Profile 8020.png</t>
+  </si>
+  <si>
+    <t>Thomas Devlin</t>
+  </si>
+  <si>
+    <t>Drop In T Nuts</t>
+  </si>
+  <si>
+    <t>20-pack drop-in t-nuts for 8020; Used for building robot and testing structures</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Abeicy-Threaded-Standard-Accessory-Extrusion/dp/B0CQT7XWTM/ref=sr_1_4?crid=2JORRM0QV185H&amp;dib=eyJ2IjoiMSJ9.AYknJgYsTETDKYCaRGfXptyIXUBLHD_-VUZwcfxyC7zIQq9SRze4m9x-GdT4X9xIfEhNncss3aBSK3NwhpisTehm480cGJBzVb1pWsAyk5k_-IjVgPHXo0KRcnRUGaRT8Pdw9l8p7yr_-oEtceDBeqhPIyUEutvoGZW9tBt6XrQZ0WFAE0U9fj6W_u8QdXAuym0pZIcUiuaWDtbpOS4HGv5gTmNo7M1_wHgrWR0maBs.aFyhF_cFf4TlCih3OW7jpfNToWRI3aKKIGCeSky1qro&amp;dib_tag=se&amp;keywords=8020+1%2F4-20+drop+in+nut+stainless&amp;qid=1756216928&amp;sprefix=8020+1%2F4-20+drop+in+nut+stainless%2Caps%2C77&amp;sr=8-4</t>
+  </si>
+  <si>
+    <t>Drop In T Nuts.png</t>
+  </si>
+  <si>
+    <t>2awg_Wire</t>
+  </si>
+  <si>
+    <t>25ft Black + Red 2awg wire. Used on all our vehicles power system; recurring yearly cost</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Welding-Battery-Copper-Flexible-Inverter/dp/B01MY9SAK1/ref=sr_1_4?crid=2C2SHCV1P266Q&amp;dib=eyJ2IjoiMSJ9.H8iAjj_Ekqmubb8AdGf5Y5p_bmiDeemqwxkAikI20hwojDjS86bfbd5X9dUrd4-8AlTdcXlxMa2Qdecsy9Read8phpg85GeVs9jS1w_461FWInIznPDnPhJZhhpR-0JAHPBH-wwBS88bSnLchYLhexrQb2vb3NPo2xzzH0XqOR5iqHgs01MBptdhXJ4M1HwR-kLfj0uCoRqHkSGjBLf01yqwD1Alu8RD2KXTwbsttHk.C-xnJqwgCwqMzl_na61P4MNCOd7S2fS4qyainL7uArs&amp;dib_tag=se&amp;keywords=2%2Bawg%2Bbattery%2Bcable%2Bwire&amp;qid=1756217344&amp;sprefix=%2Caps%2C157&amp;sr=8-4&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://gtvault.sharepoint.com/sites/MarineRoboticsGroup/Shared%20Documents/Forms/AllItems.aspx?viewid=fd287ec4%2D27e7%2D4522%2Da3ab%2Dc8258347670f&amp;id=%2Fsites%2FMarineRoboticsGroup%2FShared%20Documents%2FOPS%2D1%20Operations%2FFall%202025%20Finances%2FFall%202025%20Bill%20Proof%2FMarine%20Robotics%20Group%20Fall%202025%20Bill%20No%2E%201%2F2awg%5FWire%2Epng&amp;parent=%2Fsites%2FMarineRoboticsGroup%2FShared%20Documents%2FOPS%2D1%20Operations%2FFall%202025%20Finances%2FFall%202025%20Bill%20Proof%2FMarine%20Robotics%20Group%20Fall%202025%20Bill%20No%2E%201</t>
   </si>
   <si>
     <t>Request 1</t>
@@ -331,17 +373,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -381,6 +413,23 @@
       <fill>
         <patternFill>
           <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -724,22 +773,22 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="12" style="10" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="98.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="34.42578125" customWidth="1"/>
     <col min="13" max="13" width="16.85546875" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" customWidth="1"/>
@@ -902,15 +951,81 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5" s="7">
+        <v>21.04</v>
+      </c>
       <c r="J5" s="10">
         <f>H5*I5</f>
-        <v>0</v>
+        <v>84.16</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6" s="7">
+        <v>9.59</v>
+      </c>
       <c r="J6" s="10">
         <f>H6*I6</f>
-        <v>0</v>
+        <v>47.95</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15">
@@ -926,9 +1041,42 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9" s="7">
+        <v>146.93</v>
+      </c>
       <c r="J9" s="10">
         <f>H9*I9</f>
-        <v>0</v>
+        <v>293.86</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15">
@@ -946,7 +1094,7 @@
     <row r="12" spans="1:13" ht="15"/>
     <row r="13" spans="1:13" s="5" customFormat="1" ht="15">
       <c r="C13" s="5" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="11"/>
@@ -968,12 +1116,15 @@
     <row r="28" ht="15"/>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576 G2">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"mouser"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>"mcmaster"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"amazon"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -984,13 +1135,19 @@
     <hyperlink ref="L3" r:id="rId4" display="https://gtvault.sharepoint.com/sites/MarineRoboticsGroup/Shared%20Documents/Forms/AllItems.aspx?viewid=fd287ec4%2D27e7%2D4522%2Da3ab%2Dc8258347670f&amp;id=%2Fsites%2FMarineRoboticsGroup%2FShared%20Documents%2FOPS%2D1%20Operations%2FFall%202025%20Finances%2FFall%202025%20Bill%20Proof%2FMarine%20Robotics%20Group%20Fall%202025%20Bill%20No%2E%201%2FSolder%2Epng&amp;parent=%2Fsites%2FMarineRoboticsGroup%2FShared%20Documents%2FOPS%2D1%20Operations%2FFall%202025%20Finances%2FFall%202025%20Bill%20Proof%2FMarine%20Robotics%20Group%20Fall%202025%20Bill%20No%2E%201" xr:uid="{689A3510-645D-4C6E-86B4-66C072908384}"/>
     <hyperlink ref="L4" r:id="rId5" display="https://gtvault.sharepoint.com/sites/MarineRoboticsGroup/Shared%20Documents/Forms/AllItems.aspx?viewid=fd287ec4%2D27e7%2D4522%2Da3ab%2Dc8258347670f&amp;id=%2Fsites%2FMarineRoboticsGroup%2FShared%20Documents%2FOPS%2D1%20Operations%2FFall%202025%20Finances%2FFall%202025%20Bill%20Proof%2FMarine%20Robotics%20Group%20Fall%202025%20Bill%20No%2E%201%2FFlag%2Epng&amp;parent=%2Fsites%2FMarineRoboticsGroup%2FShared%20Documents%2FOPS%2D1%20Operations%2FFall%202025%20Finances%2FFall%202025%20Bill%20Proof%2FMarine%20Robotics%20Group%20Fall%202025%20Bill%20No%2E%201" xr:uid="{C278D17F-6DAB-4678-BB36-DB93CD0C41AD}"/>
     <hyperlink ref="K4" r:id="rId6" display="https://www.amazon.com/Waterproof-Compatible-Jackets%EF%BC%8C-University-Anniversary/dp/B0FHPP4488/ref=sr_1_20_sspa?crid=2Y8SRK5LJLYRT&amp;dib=eyJ2IjoiMSJ9.GFlDU7R-0dO02sSyXG4KHtpHMTcZaWvVdl67xPD3sjl7wjqvvvIBW0Z2ekixxIaEirwPN0IDxAIpAJjtIi5LV-UA-4WLsDfGFGJ5bwgFHpGWEoO_9DcJ0HFcxWUGOh7gZ1WVBguAahcVm4tAtM_UQJNc4ZEWYtjE6_O-Mhn5Ph09nKhVEJVoxMsYvQdjdIBqZAJq_qMlQ4S2p8lTBu8mIc6dC6niVUWR2XqWtFtv1qrahy6rXnCNEFIzFL4svnduvq2_QOn49xffSOYdMwTVqruXrwHtTMEKXPy5_AuOfSo.khrHjhdFyIOLc2a9WEbGBI0AUqDq7uoSQKbWI7g7yw8&amp;dib_tag=se&amp;keywords=georgia+tech+flag&amp;qid=1756213830&amp;sprefix=georgia+tech+flag%2Caps%2C114&amp;sr=8-20-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9tdGY&amp;psc=1" xr:uid="{B6318A0B-1C99-46F6-B118-A06DFCCFE63E}"/>
+    <hyperlink ref="K5" r:id="rId7" xr:uid="{E15B81D1-C275-42EA-B87B-889682C41EAA}"/>
+    <hyperlink ref="L5" r:id="rId8" xr:uid="{0FB383C1-D7FD-4426-A38E-31E39CF4EA0D}"/>
+    <hyperlink ref="L6" r:id="rId9" xr:uid="{54653B72-6531-4813-B990-38FFF63ED349}"/>
+    <hyperlink ref="K6" r:id="rId10" display="https://www.amazon.com/Abeicy-Threaded-Standard-Accessory-Extrusion/dp/B0CQT7XWTM/ref=sr_1_4?crid=2JORRM0QV185H&amp;dib=eyJ2IjoiMSJ9.AYknJgYsTETDKYCaRGfXptyIXUBLHD_-VUZwcfxyC7zIQq9SRze4m9x-GdT4X9xIfEhNncss3aBSK3NwhpisTehm480cGJBzVb1pWsAyk5k_-IjVgPHXo0KRcnRUGaRT8Pdw9l8p7yr_-oEtceDBeqhPIyUEutvoGZW9tBt6XrQZ0WFAE0U9fj6W_u8QdXAuym0pZIcUiuaWDtbpOS4HGv5gTmNo7M1_wHgrWR0maBs.aFyhF_cFf4TlCih3OW7jpfNToWRI3aKKIGCeSky1qro&amp;dib_tag=se&amp;keywords=8020+1%2F4-20+drop+in+nut+stainless&amp;qid=1756216928&amp;sprefix=8020+1%2F4-20+drop+in+nut+stainless%2Caps%2C77&amp;sr=8-4" xr:uid="{5F3391AB-909E-461B-B9BF-6B08EA3CE867}"/>
+    <hyperlink ref="K9" r:id="rId11" display="https://www.amazon.com/Welding-Battery-Copper-Flexible-Inverter/dp/B01MY9SAK1/ref=sr_1_4?crid=2C2SHCV1P266Q&amp;dib=eyJ2IjoiMSJ9.H8iAjj_Ekqmubb8AdGf5Y5p_bmiDeemqwxkAikI20hwojDjS86bfbd5X9dUrd4-8AlTdcXlxMa2Qdecsy9Read8phpg85GeVs9jS1w_461FWInIznPDnPhJZhhpR-0JAHPBH-wwBS88bSnLchYLhexrQb2vb3NPo2xzzH0XqOR5iqHgs01MBptdhXJ4M1HwR-kLfj0uCoRqHkSGjBLf01yqwD1Alu8RD2KXTwbsttHk.C-xnJqwgCwqMzl_na61P4MNCOd7S2fS4qyainL7uArs&amp;dib_tag=se&amp;keywords=2%2Bawg%2Bbattery%2Bcable%2Bwire&amp;qid=1756217344&amp;sprefix=%2Caps%2C157&amp;sr=8-4&amp;th=1" xr:uid="{BFF23DB3-DEDF-45FC-AD98-B27945365718}"/>
+    <hyperlink ref="L9" r:id="rId12" display="https://gtvault.sharepoint.com/sites/MarineRoboticsGroup/Shared%20Documents/Forms/AllItems.aspx?viewid=fd287ec4%2D27e7%2D4522%2Da3ab%2Dc8258347670f&amp;id=%2Fsites%2FMarineRoboticsGroup%2FShared%20Documents%2FOPS%2D1%20Operations%2FFall%202025%20Finances%2FFall%202025%20Bill%20Proof%2FMarine%20Robotics%20Group%20Fall%202025%20Bill%20No%2E%201%2F2awg%5FWire%2Epng&amp;parent=%2Fsites%2FMarineRoboticsGroup%2FShared%20Documents%2FOPS%2D1%20Operations%2FFall%202025%20Finances%2FFall%202025%20Bill%20Proof%2FMarine%20Robotics%20Group%20Fall%202025%20Bill%20No%2E%201" xr:uid="{C4AB7D65-53F3-4D01-A2AE-8B8CB13B8350}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="10" operator="equal" id="{00000000-000E-0000-0000-000004000000}">
+          <x14:cfRule type="cellIs" priority="11" operator="equal" id="{00000000-000E-0000-0000-000004000000}">
             <xm:f>Keys!$A$5</xm:f>
             <x14:dxf>
               <fill>
@@ -1000,7 +1157,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="11" operator="equal" id="{00000000-000E-0000-0000-000006000000}">
+          <x14:cfRule type="cellIs" priority="12" operator="equal" id="{00000000-000E-0000-0000-000006000000}">
             <xm:f>Keys!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1010,7 +1167,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="12" operator="equal" id="{00000000-000E-0000-0000-000007000000}">
+          <x14:cfRule type="cellIs" priority="13" operator="equal" id="{00000000-000E-0000-0000-000007000000}">
             <xm:f>Keys!$A$3</xm:f>
             <x14:dxf>
               <fill>
@@ -1020,7 +1177,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="13" operator="equal" id="{00000000-000E-0000-0000-000008000000}">
+          <x14:cfRule type="cellIs" priority="14" operator="equal" id="{00000000-000E-0000-0000-000008000000}">
             <xm:f>Keys!$A$2</xm:f>
             <x14:dxf>
               <fill>
@@ -1033,7 +1190,7 @@
           <xm:sqref>D1:D1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="14" operator="equal" id="{00000000-000E-0000-0000-000001000000}">
+          <x14:cfRule type="cellIs" priority="15" operator="equal" id="{00000000-000E-0000-0000-000001000000}">
             <xm:f>Keys!$C$3</xm:f>
             <x14:dxf>
               <fill>
@@ -1043,7 +1200,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="15" operator="equal" id="{00000000-000E-0000-0000-000002000000}">
+          <x14:cfRule type="cellIs" priority="16" operator="equal" id="{00000000-000E-0000-0000-000002000000}">
             <xm:f>Keys!$C$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1113,19 +1270,19 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1133,7 +1290,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1141,49 +1298,49 @@
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="C9" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="C10" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1193,19 +1350,19 @@
     </row>
     <row r="12" spans="1:3">
       <c r="C12" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="C14" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1215,62 +1372,62 @@
     </row>
     <row r="16" spans="1:3">
       <c r="C16" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="3:3">
       <c r="C17" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="3:3">
       <c r="C21" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="3:3">
       <c r="C22" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="3:3">
       <c r="C23" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="3:3">
       <c r="C24" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="3:3">
       <c r="C25" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="3:3">
       <c r="C26" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="3:3">
       <c r="C27" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1293,15 +1450,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <README xmlns="004ec324-7f8b-4817-8963-e485a1c8246b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="004ec324-7f8b-4817-8963-e485a1c8246b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="93d7142d-6220-43f9-a7d6-3736e306199e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1574,16 +1728,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <README xmlns="004ec324-7f8b-4817-8963-e485a1c8246b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="004ec324-7f8b-4817-8963-e485a1c8246b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="93d7142d-6220-43f9-a7d6-3736e306199e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E184BB0C-9F34-433E-977A-8C3E17A4E2AB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5CA8B09-733A-4EB5-9269-52554A3D84A2}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1591,5 +1748,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5CA8B09-733A-4EB5-9269-52554A3D84A2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E184BB0C-9F34-433E-977A-8C3E17A4E2AB}"/>
 </file>
</xml_diff>